<commit_message>
All scenar (no test)
Без 5
</commit_message>
<xml_diff>
--- a/Шаблоны/Scenar8.xlsx
+++ b/Шаблоны/Scenar8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="233">
   <si>
     <t>Дата прохождения:</t>
   </si>
@@ -719,15 +719,9 @@
     <t>Произвести осмотр опорно-стержневой изоляции ЛР 110 Заря.</t>
   </si>
   <si>
-    <t>ОРУ_110_ЛР110_Заря_БлокировочныйКлюч</t>
-  </si>
-  <si>
     <t>Вставить деблокировочный ключ в замок ЛР 110 Заря</t>
   </si>
   <si>
-    <t>Кнопкой с блока управления отключить ЛР 110 Заря.</t>
-  </si>
-  <si>
     <t>Визуально убедиться в отключенном положении ЛР 110 Заря.</t>
   </si>
   <si>
@@ -737,15 +731,6 @@
     <t>На привод ЛР 110 Заря вывесить плакат «НЕ ВКЛЮЧАТЬ! Работают люди».</t>
   </si>
   <si>
-    <t>ОРУ_110_Автомат_ЛР110_Т1</t>
-  </si>
-  <si>
-    <t>Отключить автомат цепей питания привода ЛР 110 Т1.</t>
-  </si>
-  <si>
-    <t>ОРУ_110_Плакат_ЛР110</t>
-  </si>
-  <si>
     <t>На автомат цепей питания привода ЛР 110 Заря вывесить плакат «НЕ ВКЛЮЧАТЬ! работают люди».</t>
   </si>
   <si>
@@ -755,15 +740,9 @@
     <t>Произвести осмотр опорно-стержневой изоляции ШР 110 Заря.</t>
   </si>
   <si>
-    <t>ОРУ_110_ШР110_Заря_БлокировочныйКлюч</t>
-  </si>
-  <si>
     <t>Вставить деблокировочный ключ в замок ШР 110 Заря.</t>
   </si>
   <si>
-    <t>Кнопкой с блока управления отключить ШР 110 Заря.</t>
-  </si>
-  <si>
     <t>ОРУ_110_Плакат_ШР110</t>
   </si>
   <si>
@@ -776,9 +755,6 @@
     <t>Отключить автомат цепей питания привода ШР 110 Заря.</t>
   </si>
   <si>
-    <t>ОРУ_110_Плакат_ШР110_Заря</t>
-  </si>
-  <si>
     <t>На автомат цепей питания привода ШР 110 Заря вывесить плакат «НЕ ВКЛЮЧАТЬ! работают люди».</t>
   </si>
   <si>
@@ -788,9 +764,6 @@
     <t>Взять указатель напряжения 110 кВ.</t>
   </si>
   <si>
-    <t>ОРУ_110_Указатель_110кВ</t>
-  </si>
-  <si>
     <t>Проверить исправность указателя напряжения 110 кВ, прикосновением к токоведущим частям, заведомо находящимся под напряжением - к жесткой ошиновке 110 кВ.</t>
   </si>
   <si>
@@ -800,9 +773,6 @@
     <t>Осмотреть опорно-стержневую изоляцию ЗНВ ЛР 110 Заря.</t>
   </si>
   <si>
-    <t>ОРУ_110_БлокировочныйКлюч</t>
-  </si>
-  <si>
     <t>Вставить деблокировочный ключ</t>
   </si>
   <si>
@@ -818,12 +788,6 @@
     <t>Включить ЗНВ ШР 110 Заря.</t>
   </si>
   <si>
-    <t>ОРУ_110_ЗОН110_Т1</t>
-  </si>
-  <si>
-    <t>ОРУ_110_Перчатки_Проверить</t>
-  </si>
-  <si>
     <t>Отключить ЗОН 110 Т1.</t>
   </si>
   <si>
@@ -837,6 +801,57 @@
   </si>
   <si>
     <t>Визуально проверить отключенное состояние ЗОН 110 Т2.</t>
+  </si>
+  <si>
+    <t>Ключом с блока управления отключить ЛР 110 Заря.</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЛР110_Заря_ДеблокировочныйКлюч</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЛР110_Заря_Ключ</t>
+  </si>
+  <si>
+    <t>ОРУ_110_Автомат_ЛР110_Заря</t>
+  </si>
+  <si>
+    <t>Отключить автомат цепей питания привода ЛР 110 Заря.</t>
+  </si>
+  <si>
+    <t>ОРУ_110_Плакат_Автомат_ЛР110_Заря</t>
+  </si>
+  <si>
+    <t>Ключом с блока управления отключить ШР 110 Заря.</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ШР110_Заря_Ключ</t>
+  </si>
+  <si>
+    <t>Визуально убедиться в отключенном положении ШР 110 Заря.</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ШР110_Заря_ДеблокировочныйКлюч</t>
+  </si>
+  <si>
+    <t>ОРУ_110_Плакат_Автомат_ШР110_Заря</t>
+  </si>
+  <si>
+    <t>ОРУ110_110кВ_2секция</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЗНВ_ЛР110_ДеблокировочныйКлюч</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЗНВ_ЛР110_Заря</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЗНВ_ШР110_Заря</t>
+  </si>
+  <si>
+    <t>Визуально проверить включенное положение ЗНВ ШР 110 Заря.</t>
+  </si>
+  <si>
+    <t>ОРУ_110_ЗНВ_ШР110_ДеблокировочныйКлюч</t>
   </si>
 </sst>
 </file>
@@ -846,12 +861,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -946,6 +969,12 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -994,55 +1023,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1350,7 +1387,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45509</v>
+        <v>45524</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,448 +1477,560 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B143"/>
+  <dimension ref="B1:F143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="25"/>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="25"/>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="25"/>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="25"/>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="25"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="25"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="25"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="25"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="25"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="25"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="25"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="25"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="25"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="25"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="25"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="25"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="25"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="25"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="25"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="25"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="25"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="25"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="25"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="25"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="25"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="25"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="25"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="25"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="25"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="25"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="25"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="25"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="25"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="25"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="25"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="25"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="25"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="25"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="25"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="25"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="25"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="25"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="25"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="25"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="25"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="25"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="25"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="25"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="25"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="25"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="25"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="25"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="25"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="25"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="25"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="25"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="25"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="25"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="25"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="25"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="25"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="25"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="25"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="25"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="25"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="25"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="25"/>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="23"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+      <c r="F9" s="27"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="23"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="23"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="23"/>
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="23"/>
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="23"/>
+      <c r="F23" s="27"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+      <c r="F24" s="27"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
+      <c r="F25" s="27"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="23"/>
+      <c r="F27" s="27"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="23"/>
+      <c r="F28" s="27"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="23"/>
+      <c r="F29" s="27"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="23"/>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="23"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="23"/>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="23"/>
+      <c r="F33" s="27"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="23"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="23"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="23"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="23"/>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="23"/>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="23"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="23"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="23"/>
+      <c r="F41" s="27"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="23"/>
+      <c r="F42" s="27"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="23"/>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+      <c r="F44" s="27"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="23"/>
+      <c r="F47" s="27"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="23"/>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="23"/>
+      <c r="F49" s="27"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="23"/>
+      <c r="F50" s="27"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="23"/>
+      <c r="F51" s="27"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="23"/>
+      <c r="F52" s="27"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="23"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="23"/>
+      <c r="F54" s="27"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="23"/>
+      <c r="F55" s="27"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="23"/>
+      <c r="F56" s="27"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="23"/>
+      <c r="F57" s="27"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="23"/>
+      <c r="F58" s="27"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="23"/>
+      <c r="F59" s="27"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="23"/>
+      <c r="F60" s="27"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="23"/>
+      <c r="F61" s="27"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="23"/>
+      <c r="F62" s="27"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="23"/>
+      <c r="F63" s="27"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="23"/>
+      <c r="F64" s="27"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="23"/>
+      <c r="F65" s="27"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="23"/>
+      <c r="F66" s="27"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="23"/>
+      <c r="F67" s="27"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="23"/>
+      <c r="F68" s="27"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="23"/>
+      <c r="F69" s="27"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="23"/>
+      <c r="F70" s="27"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="23"/>
+      <c r="F71" s="27"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="23"/>
+      <c r="F72" s="27"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="23"/>
+      <c r="F73" s="27"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="23"/>
+      <c r="F74" s="27"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="23"/>
+      <c r="F75" s="27"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="23"/>
+      <c r="F76" s="27"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="23"/>
+      <c r="F77" s="27"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="23"/>
+      <c r="F78" s="27"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="23"/>
+      <c r="F79" s="27"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="23"/>
+      <c r="F80" s="27"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="23"/>
+      <c r="F81" s="27"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="23"/>
+      <c r="F82" s="27"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="23"/>
+      <c r="F83" s="27"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="23"/>
+      <c r="F84" s="27"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="23"/>
+      <c r="F85" s="27"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="23"/>
+      <c r="F86" s="27"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="23"/>
+      <c r="F87" s="27"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="23"/>
+      <c r="F88" s="27"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="23"/>
+      <c r="F89" s="27"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="23"/>
+      <c r="F90" s="27"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="23"/>
+      <c r="F91" s="27"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="23"/>
+      <c r="F92" s="27"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="23"/>
+      <c r="F93" s="27"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="23"/>
+      <c r="F94" s="27"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="23"/>
+      <c r="F95" s="27"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="23"/>
+      <c r="F96" s="27"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="23"/>
+      <c r="F97" s="27"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="23"/>
+      <c r="F98" s="27"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="23"/>
+      <c r="F99" s="27"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="23"/>
+      <c r="F100" s="27"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="23"/>
+      <c r="F101" s="27"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="23"/>
+      <c r="F102" s="27"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="23"/>
+      <c r="F103" s="27"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="23"/>
+      <c r="F104" s="27"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="23"/>
+      <c r="F105" s="27"/>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="23"/>
+      <c r="F106" s="27"/>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="23"/>
+      <c r="F107" s="27"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B108" s="23"/>
+      <c r="F108" s="27"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B109" s="23"/>
+      <c r="F109" s="27"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B110" s="23"/>
+      <c r="F110" s="27"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="23"/>
+      <c r="F111" s="27"/>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="23"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="25"/>
+      <c r="B113" s="23"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="25"/>
+      <c r="B114" s="23"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="25"/>
+      <c r="B115" s="23"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="25"/>
+      <c r="B116" s="23"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="25"/>
+      <c r="B117" s="23"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="25"/>
+      <c r="B118" s="23"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="25"/>
+      <c r="B119" s="23"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="25"/>
+      <c r="B120" s="23"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="25"/>
+      <c r="B121" s="23"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="25"/>
+      <c r="B122" s="23"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="25"/>
+      <c r="B123" s="23"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="25"/>
+      <c r="B124" s="23"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="25"/>
+      <c r="B125" s="23"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="25"/>
+      <c r="B126" s="23"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="25"/>
+      <c r="B127" s="23"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="25"/>
+      <c r="B128" s="23"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="25"/>
+      <c r="B129" s="23"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="25"/>
+      <c r="B130" s="23"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="25"/>
+      <c r="B131" s="23"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="25"/>
+      <c r="B132" s="23"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="25"/>
+      <c r="B133" s="23"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="25"/>
+      <c r="B134" s="23"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="25"/>
+      <c r="B135" s="23"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="25"/>
+      <c r="B136" s="23"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="25"/>
+      <c r="B137" s="23"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="25"/>
+      <c r="B138" s="23"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="25"/>
+      <c r="B139" s="23"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="25"/>
+      <c r="B140" s="23"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="25"/>
+      <c r="B141" s="23"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="25"/>
+      <c r="B142" s="23"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="25"/>
+      <c r="B143" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1890,15 +2039,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K132"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
@@ -3738,10 +3887,12 @@
       <c r="C90" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E90" s="9"/>
+      <c r="D90" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="9">
+        <v>1</v>
+      </c>
       <c r="F90" s="14" t="s">
         <v>187</v>
       </c>
@@ -3796,15 +3947,15 @@
         <v>92</v>
       </c>
       <c r="B93" s="9"/>
-      <c r="C93" s="20" t="s">
-        <v>188</v>
+      <c r="C93" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E93" s="9"/>
-      <c r="F93" s="21" t="s">
-        <v>189</v>
+      <c r="F93" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="G93" s="18" t="s">
         <v>32</v>
@@ -3815,15 +3966,17 @@
         <v>93</v>
       </c>
       <c r="B94" s="9"/>
-      <c r="C94" s="20" t="s">
-        <v>186</v>
+      <c r="C94" s="24" t="s">
+        <v>218</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E94" s="9"/>
+      <c r="E94" s="9">
+        <v>1</v>
+      </c>
       <c r="F94" s="14" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>31</v>
@@ -3834,15 +3987,17 @@
         <v>94</v>
       </c>
       <c r="B95" s="9"/>
-      <c r="C95" s="20" t="s">
+      <c r="C95" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E95" s="9"/>
-      <c r="F95" s="22" t="s">
-        <v>191</v>
+      <c r="D95" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E95" s="9">
+        <v>2</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="G95" s="16" t="s">
         <v>33</v>
@@ -3853,15 +4008,15 @@
         <v>95</v>
       </c>
       <c r="B96" s="9"/>
-      <c r="C96" s="20" t="s">
-        <v>192</v>
+      <c r="C96" s="24" t="s">
+        <v>190</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E96" s="9"/>
       <c r="F96" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G96" s="15" t="s">
         <v>34</v>
@@ -3873,14 +4028,16 @@
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="10" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E97" s="9"/>
+      <c r="E97" s="9">
+        <v>1</v>
+      </c>
       <c r="F97" s="14" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="G97" s="15" t="s">
         <v>34</v>
@@ -3892,14 +4049,14 @@
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="10" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="D98" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E98" s="9"/>
       <c r="F98" s="14" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G98" s="15" t="s">
         <v>34</v>
@@ -3911,14 +4068,16 @@
       </c>
       <c r="B99" s="9"/>
       <c r="C99" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E99" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="E99" s="9">
+        <v>1</v>
+      </c>
       <c r="F99" s="14" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G99" s="16" t="s">
         <v>33</v>
@@ -3972,14 +4131,14 @@
       </c>
       <c r="B102" s="9"/>
       <c r="C102" s="10" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E102" s="9"/>
-      <c r="F102" s="21" t="s">
-        <v>201</v>
+      <c r="F102" s="20" t="s">
+        <v>195</v>
       </c>
       <c r="G102" s="18" t="s">
         <v>32</v>
@@ -3991,113 +4150,117 @@
       </c>
       <c r="B103" s="9"/>
       <c r="C103" s="10" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E103" s="9"/>
-      <c r="F103" s="21" t="s">
-        <v>202</v>
+        <v>41</v>
+      </c>
+      <c r="E103" s="9">
+        <v>1</v>
+      </c>
+      <c r="F103" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="G103" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>103</v>
       </c>
       <c r="B104" s="9"/>
       <c r="C104" s="10" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E104" s="9"/>
-      <c r="F104" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="G104" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E104" s="9">
+        <v>2</v>
+      </c>
+      <c r="F104" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G104" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>104</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>37</v>
+        <v>196</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="E105" s="9"/>
-      <c r="F105" s="21" t="s">
-        <v>206</v>
+      <c r="F105" s="20" t="s">
+        <v>197</v>
       </c>
       <c r="G105" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>105</v>
       </c>
       <c r="B106" s="9"/>
       <c r="C106" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E106" s="9"/>
-      <c r="F106" s="21" t="s">
-        <v>208</v>
+        <v>198</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E106" s="9">
+        <v>1</v>
+      </c>
+      <c r="F106" s="20" t="s">
+        <v>199</v>
       </c>
       <c r="G106" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>106</v>
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D107" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E107" s="9">
-        <v>6</v>
-      </c>
-      <c r="F107" s="14" t="s">
-        <v>30</v>
+        <v>226</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E107" s="9"/>
+      <c r="F107" s="20" t="s">
+        <v>200</v>
       </c>
       <c r="G107" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>107</v>
       </c>
       <c r="B108" s="9"/>
       <c r="C108" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D108" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E108" s="9">
         <v>6</v>
       </c>
-      <c r="F108" s="21" t="s">
-        <v>29</v>
+      <c r="F108" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>34</v>
@@ -4109,14 +4272,16 @@
       </c>
       <c r="B109" s="9"/>
       <c r="C109" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E109" s="23"/>
-      <c r="F109" s="21" t="s">
-        <v>210</v>
+        <v>51</v>
+      </c>
+      <c r="D109" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E109" s="9">
+        <v>6</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="G109" s="15" t="s">
         <v>34</v>
@@ -4128,14 +4293,14 @@
       </c>
       <c r="B110" s="9"/>
       <c r="C110" s="10" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E110" s="9"/>
-      <c r="F110" s="24" t="s">
-        <v>212</v>
+      <c r="F110" s="22" t="s">
+        <v>203</v>
       </c>
       <c r="G110" s="15" t="s">
         <v>34</v>
@@ -4147,14 +4312,14 @@
       </c>
       <c r="B111" s="9"/>
       <c r="C111" s="10" t="s">
-        <v>65</v>
+        <v>186</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E111" s="9"/>
-      <c r="F111" s="24" t="s">
-        <v>213</v>
+      <c r="F111" s="22" t="s">
+        <v>204</v>
       </c>
       <c r="G111" s="15" t="s">
         <v>34</v>
@@ -4166,14 +4331,16 @@
       </c>
       <c r="B112" s="9"/>
       <c r="C112" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E112" s="9"/>
-      <c r="F112" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
+      </c>
+      <c r="D112" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E112" s="9">
+        <v>1</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>205</v>
       </c>
       <c r="G112" s="16" t="s">
         <v>33</v>
@@ -4185,14 +4352,14 @@
       </c>
       <c r="B113" s="9"/>
       <c r="C113" s="10" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E113" s="9"/>
-      <c r="F113" s="21" t="s">
-        <v>216</v>
+      <c r="F113" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="G113" s="18" t="s">
         <v>32</v>
@@ -4204,14 +4371,16 @@
       </c>
       <c r="B114" s="9"/>
       <c r="C114" s="10" t="s">
-        <v>186</v>
+        <v>229</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E114" s="9"/>
-      <c r="F114" s="21" t="s">
-        <v>217</v>
+      <c r="E114" s="9">
+        <v>2</v>
+      </c>
+      <c r="F114" s="20" t="s">
+        <v>207</v>
       </c>
       <c r="G114" s="13" t="s">
         <v>31</v>
@@ -4223,14 +4392,16 @@
       </c>
       <c r="B115" s="9"/>
       <c r="C115" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E115" s="9"/>
-      <c r="F115" s="21" t="s">
-        <v>218</v>
+        <v>229</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E115" s="9">
+        <v>2</v>
+      </c>
+      <c r="F115" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="G115" s="16" t="s">
         <v>33</v>
@@ -4271,7 +4442,7 @@
       <c r="E117" s="9">
         <v>7</v>
       </c>
-      <c r="F117" s="21" t="s">
+      <c r="F117" s="20" t="s">
         <v>29</v>
       </c>
       <c r="G117" s="15" t="s">
@@ -4284,14 +4455,14 @@
       </c>
       <c r="B118" s="9"/>
       <c r="C118" s="10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E118" s="9"/>
-      <c r="F118" s="21" t="s">
-        <v>210</v>
+      <c r="F118" s="20" t="s">
+        <v>202</v>
       </c>
       <c r="G118" s="15" t="s">
         <v>34</v>
@@ -4303,14 +4474,14 @@
       </c>
       <c r="B119" s="9"/>
       <c r="C119" s="10" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E119" s="9"/>
-      <c r="F119" s="24" t="s">
-        <v>212</v>
+      <c r="F119" s="22" t="s">
+        <v>203</v>
       </c>
       <c r="G119" s="15" t="s">
         <v>34</v>
@@ -4322,14 +4493,16 @@
       </c>
       <c r="B120" s="9"/>
       <c r="C120" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D120" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E120" s="9"/>
-      <c r="F120" s="21" t="s">
-        <v>219</v>
+        <v>230</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E120" s="9">
+        <v>1</v>
+      </c>
+      <c r="F120" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="G120" s="16" t="s">
         <v>33</v>
@@ -4341,14 +4514,14 @@
       </c>
       <c r="B121" s="9"/>
       <c r="C121" s="10" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E121" s="9"/>
-      <c r="F121" s="21" t="s">
-        <v>216</v>
+      <c r="F121" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="G121" s="18" t="s">
         <v>32</v>
@@ -4360,14 +4533,16 @@
       </c>
       <c r="B122" s="9"/>
       <c r="C122" s="10" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E122" s="9"/>
+      <c r="E122" s="9">
+        <v>2</v>
+      </c>
       <c r="F122" s="14" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G122" s="13" t="s">
         <v>31</v>
@@ -4379,17 +4554,19 @@
       </c>
       <c r="B123" s="9"/>
       <c r="C123" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D123" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E123" s="9"/>
-      <c r="F123" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G123" s="15" t="s">
-        <v>34</v>
+        <v>230</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E123" s="9">
+        <v>2</v>
+      </c>
+      <c r="F123" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="G123" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4398,33 +4575,37 @@
       </c>
       <c r="B124" s="9"/>
       <c r="C124" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D124" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E124" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E124" s="9">
+        <v>3</v>
+      </c>
       <c r="F124" s="14" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="G124" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>124</v>
       </c>
       <c r="B125" s="9"/>
       <c r="C125" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D125" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E125" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="E125" s="9">
+        <v>8</v>
+      </c>
       <c r="F125" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G125" s="15" t="s">
         <v>34</v>
@@ -4436,36 +4617,40 @@
       </c>
       <c r="B126" s="9"/>
       <c r="C126" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D126" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E126" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="D126" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E126" s="9">
+        <v>8</v>
+      </c>
       <c r="F126" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="G126" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G126" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>126</v>
       </c>
       <c r="B127" s="9"/>
       <c r="C127" s="10" t="s">
-        <v>221</v>
+        <v>85</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E127" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="E127" s="9">
+        <v>1</v>
+      </c>
       <c r="F127" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="G127" s="16" t="s">
-        <v>33</v>
+        <v>211</v>
+      </c>
+      <c r="G127" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4474,17 +4659,19 @@
       </c>
       <c r="B128" s="9"/>
       <c r="C128" s="10" t="s">
-        <v>225</v>
+        <v>83</v>
       </c>
       <c r="D128" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E128" s="9"/>
+      <c r="E128" s="9">
+        <v>4</v>
+      </c>
       <c r="F128" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G128" s="15" t="s">
-        <v>34</v>
+        <v>212</v>
+      </c>
+      <c r="G128" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4493,37 +4680,37 @@
       </c>
       <c r="B129" s="9"/>
       <c r="C129" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D129" s="17" t="s">
-        <v>44</v>
+        <v>92</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="E129" s="9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F129" s="14" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="G129" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>129</v>
       </c>
       <c r="B130" s="9"/>
       <c r="C130" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D130" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E130" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F130" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G130" s="15" t="s">
         <v>34</v>
@@ -4535,40 +4722,65 @@
       </c>
       <c r="B131" s="9"/>
       <c r="C131" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="D131" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E131" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="D131" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E131" s="9">
+        <v>9</v>
+      </c>
       <c r="F131" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="G131" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G131" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>131</v>
       </c>
       <c r="B132" s="9"/>
       <c r="C132" s="10" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E132" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="E132" s="9">
+        <v>1</v>
+      </c>
       <c r="F132" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G132" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="G132" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="9">
+        <v>132</v>
+      </c>
+      <c r="B133" s="9"/>
+      <c r="C133" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E133" s="9">
+        <v>4</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="G133" s="16" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>